<commit_message>
Ajustes vista inventarios y importacion
</commit_message>
<xml_diff>
--- a/planning/assets/formatsXlsx/Materia_prima.xlsx
+++ b/planning/assets/formatsXlsx/Materia_prima.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>referencia</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>unidad</t>
+  </si>
+  <si>
+    <t>cantidad</t>
   </si>
 </sst>
 </file>
@@ -57,7 +60,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -130,11 +133,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -145,20 +170,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
     <dxf>
       <font>
         <strike val="0"/>
@@ -171,12 +202,16 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -191,7 +226,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -206,7 +240,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -231,7 +264,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -257,6 +289,23 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <top/>
       </border>
     </dxf>
     <dxf>
@@ -294,11 +343,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:C6" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <tableColumns count="4">
     <tableColumn id="1" name="referencia" dataDxfId="3"/>
     <tableColumn id="2" name="material" dataDxfId="2"/>
     <tableColumn id="3" name="unidad" dataDxfId="1"/>
+    <tableColumn id="4" name="cantidad" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -589,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -600,9 +650,10 @@
     <col min="1" max="1" width="34.140625" customWidth="1"/>
     <col min="2" max="2" width="41.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:4" ht="18">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -612,31 +663,39 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="4"/>
+      <c r="D2" s="8"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="4"/>
       <c r="B6" s="6"/>
       <c r="C6" s="4"/>
+      <c r="D6" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>